<commit_message>
Fixed issue with Randic index
</commit_message>
<xml_diff>
--- a/test/reference.xlsx
+++ b/test/reference.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26207"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prismane/Documents/Github/molecules/test/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13660" windowHeight="13720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15820" windowHeight="13300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="147">
   <si>
     <t>CCCCC</t>
   </si>
@@ -420,20 +426,57 @@
     <t>Harary</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Balaban</t>
+  </si>
+  <si>
+    <t>Platt</t>
+  </si>
+  <si>
+    <t>Randic</t>
+  </si>
+  <si>
+    <t>Szeged</t>
+  </si>
+  <si>
+    <t>Marvin</t>
+  </si>
+  <si>
+    <t>mol.js</t>
+  </si>
+  <si>
+    <t>Wiener Polarity</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>C10H18O2</t>
+  </si>
+  <si>
+    <t>C6H13NO2</t>
+  </si>
+  <si>
+    <t>C7H15ClO</t>
+  </si>
+  <si>
+    <t>C9H14O2</t>
+  </si>
+  <si>
+    <t>C10H17ClO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -469,6 +512,30 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -478,7 +545,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -486,8 +553,122 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="179">
+  <cellStyleXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -667,8 +848,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -682,17 +867,98 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="179">
+  <cellStyles count="183">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -782,6 +1048,8 @@
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -871,10 +1139,17 @@
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1200,32 +1475,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U63"/>
+  <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P21" sqref="P21"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.6640625" style="1" customWidth="1"/>
     <col min="2" max="10" width="4" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.6640625" style="7" customWidth="1"/>
-    <col min="12" max="12" width="5.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="5.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5" style="1" customWidth="1"/>
-    <col min="16" max="16" width="5.6640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="6.5" style="7" customWidth="1"/>
-    <col min="18" max="18" width="5.6640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="63.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="9.83203125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.6640625" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="4" customFormat="1">
+    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>75</v>
       </c>
@@ -1256,33 +1524,20 @@
       <c r="J1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="R1" s="5"/>
-      <c r="S1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="T1" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="U1" s="4" t="s">
+      <c r="M1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1313,41 +1568,20 @@
       <c r="J2" s="1">
         <v>0</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="6">
         <v>72.150999999999996</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M2" s="1">
-        <v>20</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="O2" s="1">
-        <v>35</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q2" s="7">
-        <v>6.42</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="U2" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
+      <c r="N2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1378,41 +1612,20 @@
       <c r="J3" s="1">
         <v>0</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="6">
         <v>72.150999999999996</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M3" s="1">
-        <v>18</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="O3" s="1">
-        <v>28</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q3" s="7">
-        <v>6.67</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S3" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1443,41 +1656,20 @@
       <c r="J4" s="1">
         <v>0</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="6">
         <v>72.150999999999996</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M4" s="1">
-        <v>16</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="O4" s="1">
-        <v>22</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q4" s="7">
-        <v>7</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S4" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1508,41 +1700,20 @@
       <c r="J5" s="1">
         <v>0</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="6">
         <v>56.107999999999997</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M5" s="1">
-        <v>10</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="O5" s="1">
-        <v>15</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q5" s="7">
-        <v>4.33</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S5" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1573,41 +1744,20 @@
       <c r="J6" s="1">
         <v>0</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="6">
         <v>56.107999999999997</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M6" s="1">
-        <v>10</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="O6" s="1">
-        <v>15</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q6" s="7">
-        <v>4.33</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S6" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="U6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1638,41 +1788,20 @@
       <c r="J7" s="1">
         <v>0</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="6">
         <v>56.107999999999997</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M7" s="1">
-        <v>10</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="O7" s="1">
-        <v>15</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q7" s="7">
-        <v>4.33</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S7" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="U7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1703,41 +1832,20 @@
       <c r="J8" s="1">
         <v>0</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="6">
         <v>56.107999999999997</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M8" s="1">
-        <v>10</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="O8" s="1">
-        <v>15</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q8" s="7">
-        <v>4.33</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S8" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1768,41 +1876,20 @@
       <c r="J9" s="1">
         <v>0</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="6">
         <v>54.091999999999999</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M9" s="1">
-        <v>10</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="O9" s="1">
-        <v>15</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q9" s="7">
-        <v>4.33</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S9" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="U9" s="2" t="s">
+      <c r="N9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1833,41 +1920,20 @@
       <c r="J10" s="1">
         <v>0</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="6">
         <v>54.091999999999999</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M10" s="1">
-        <v>10</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="O10" s="1">
-        <v>15</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q10" s="7">
-        <v>4.33</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S10" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="U10" s="2" t="s">
+      <c r="N10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1898,41 +1964,20 @@
       <c r="J11" s="1">
         <v>0</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="6">
         <v>54.091999999999999</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M11" s="1">
-        <v>10</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="O11" s="1">
-        <v>15</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q11" s="7">
-        <v>4.33</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S11" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="U11" s="2" t="s">
+      <c r="N11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1963,41 +2008,20 @@
       <c r="J12" s="1">
         <v>0</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="6">
         <v>54.091999999999999</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M12" s="1">
+        <v>115</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="O12" s="1">
-        <v>15</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q12" s="7">
-        <v>4.33</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2028,41 +2052,20 @@
       <c r="J13" s="1">
         <v>0</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="6">
         <v>74.123000000000005</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M13" s="1">
-        <v>20</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="O13" s="1">
-        <v>35</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q13" s="7">
-        <v>6.42</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S13" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="T13" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="U13" s="2" t="s">
+      <c r="N13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2093,41 +2096,20 @@
       <c r="J14" s="1">
         <v>0</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="6">
         <v>74.123000000000005</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M14" s="1">
-        <v>18</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="O14" s="1">
-        <v>28</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q14" s="7">
-        <v>6.67</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S14" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="T14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="U14" s="2" t="s">
+      <c r="N14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2158,41 +2140,20 @@
       <c r="J15" s="1">
         <v>0</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="6">
         <v>74.123000000000005</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M15" s="1">
-        <v>16</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="O15" s="1">
-        <v>22</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q15" s="7">
-        <v>7</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S15" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="T15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="U15" s="2" t="s">
+      <c r="N15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2223,41 +2184,20 @@
       <c r="J16" s="1">
         <v>0</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="6">
         <v>72.106999999999999</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M16" s="1">
-        <v>20</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="O16" s="1">
-        <v>35</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q16" s="7">
-        <v>6.42</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S16" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="T16" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="U16" s="2" t="s">
+      <c r="N16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2288,23 +2228,20 @@
       <c r="J17" s="1">
         <v>0</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="6">
         <v>72.106999999999999</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S17" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="T17" s="3" t="s">
+      <c r="M17" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="U17" s="2" t="s">
+      <c r="N17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2335,23 +2272,20 @@
       <c r="J18" s="1">
         <v>0</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K18" s="6">
         <v>88.105999999999995</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S18" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="T18" s="3" t="s">
+      <c r="M18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="U18" s="2" t="s">
+      <c r="N18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2382,23 +2316,20 @@
       <c r="J19" s="1">
         <v>0</v>
       </c>
-      <c r="K19" s="7">
+      <c r="K19" s="6">
         <v>88.105999999999995</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S19" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="T19" s="3" t="s">
+      <c r="M19" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="U19" s="2" t="s">
+      <c r="N19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2429,23 +2360,20 @@
       <c r="J20" s="1">
         <v>0</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="6">
         <v>87.122</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S20" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="T20" s="3" t="s">
+      <c r="M20" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="U20" s="2" t="s">
+      <c r="N20" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2476,23 +2404,20 @@
       <c r="J21" s="1">
         <v>0</v>
       </c>
-      <c r="K21" s="7">
+      <c r="K21" s="6">
         <v>104.105</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S21" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="T21" s="3" t="s">
+      <c r="M21" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="U21" s="2" t="s">
+      <c r="N21" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2514,32 +2439,29 @@
       <c r="G22" s="1">
         <v>1</v>
       </c>
-      <c r="H22" s="6">
-        <v>0</v>
-      </c>
-      <c r="I22" s="6">
-        <v>0</v>
-      </c>
-      <c r="J22" s="6">
-        <v>0</v>
-      </c>
-      <c r="K22" s="7">
+      <c r="H22" s="5">
+        <v>0</v>
+      </c>
+      <c r="I22" s="5">
+        <v>0</v>
+      </c>
+      <c r="J22" s="5">
+        <v>0</v>
+      </c>
+      <c r="K22" s="6">
         <v>106.54900000000001</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S22" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="T22" s="1" t="s">
+      <c r="M22" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="U22" s="2" t="s">
+      <c r="N22" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2570,23 +2492,20 @@
       <c r="J23" s="1">
         <v>0</v>
       </c>
-      <c r="K23" s="7">
+      <c r="K23" s="6">
         <v>116.116</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S23" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="T23" s="1" t="s">
+      <c r="M23" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="U23" s="2" t="s">
+      <c r="N23" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2617,23 +2536,20 @@
       <c r="J24" s="1">
         <v>0</v>
       </c>
-      <c r="K24" s="7">
+      <c r="K24" s="6">
         <v>84.162000000000006</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S24" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="T24" s="1" t="s">
+      <c r="M24" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U24" s="2" t="s">
+      <c r="N24" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2664,23 +2580,20 @@
       <c r="J25" s="1">
         <v>0</v>
       </c>
-      <c r="K25" s="7">
+      <c r="K25" s="6">
         <v>166.30799999999999</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S25" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="T25" s="1" t="s">
+      <c r="M25" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="U25" s="2" t="s">
+      <c r="N25" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2711,23 +2624,20 @@
       <c r="J26" s="1">
         <v>0</v>
       </c>
-      <c r="K26" s="7">
+      <c r="K26" s="6">
         <v>152.28100000000001</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S26" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="T26" s="1" t="s">
+      <c r="M26" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="U26" s="2" t="s">
+      <c r="N26" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2758,23 +2668,20 @@
       <c r="J27" s="1">
         <v>0</v>
       </c>
-      <c r="K27" s="7">
+      <c r="K27" s="6">
         <v>80.13</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S27" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="T27" s="1" t="s">
+      <c r="M27" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U27" s="2" t="s">
+      <c r="N27" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2805,23 +2712,20 @@
       <c r="J28" s="1">
         <v>0</v>
       </c>
-      <c r="K28" s="7">
+      <c r="K28" s="6">
         <v>104.152</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S28" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="T28" s="1" t="s">
+      <c r="M28" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="U28" s="2" t="s">
+      <c r="N28" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2852,23 +2756,20 @@
       <c r="J29" s="1">
         <v>0</v>
       </c>
-      <c r="K29" s="7">
+      <c r="K29" s="6">
         <v>78.114000000000004</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S29" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="T29" s="1" t="s">
+      <c r="M29" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U29" s="2" t="s">
+      <c r="N29" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2899,23 +2800,20 @@
       <c r="J30" s="1">
         <v>0</v>
       </c>
-      <c r="K30" s="7">
+      <c r="K30" s="6">
         <v>108.14</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S30" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="T30" s="1" t="s">
+      <c r="M30" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="U30" s="2" t="s">
+      <c r="N30" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2946,23 +2844,20 @@
       <c r="J31" s="1">
         <v>0</v>
       </c>
-      <c r="K31" s="7">
+      <c r="K31" s="6">
         <v>154.21199999999999</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S31" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="T31" s="1" t="s">
+      <c r="M31" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="U31" s="2" t="s">
+      <c r="N31" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2993,23 +2888,20 @@
       <c r="J32" s="1">
         <v>0</v>
       </c>
-      <c r="K32" s="7">
+      <c r="K32" s="6">
         <v>178.22300000000001</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S32" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="T32" s="1" t="s">
+      <c r="M32" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="U32" s="2" t="s">
+      <c r="N32" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:21">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -3040,23 +2932,20 @@
       <c r="J33" s="1">
         <v>0</v>
       </c>
-      <c r="K33" s="7">
+      <c r="K33" s="6">
         <v>67.090999999999994</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S33" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="T33" s="1" t="s">
+      <c r="M33" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="U33" s="2" t="s">
+      <c r="N33" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:21">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -3087,23 +2976,20 @@
       <c r="J34" s="1">
         <v>0</v>
       </c>
-      <c r="K34" s="7">
+      <c r="K34" s="6">
         <v>68.075000000000003</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S34" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="T34" s="1" t="s">
+      <c r="M34" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="U34" s="2" t="s">
+      <c r="N34" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -3134,23 +3020,20 @@
       <c r="J35" s="1">
         <v>0</v>
       </c>
-      <c r="K35" s="7">
+      <c r="K35" s="6">
         <v>84.135999999999996</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S35" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="T35" s="1" t="s">
+      <c r="M35" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="U35" s="2" t="s">
+      <c r="N35" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:21">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -3181,23 +3064,20 @@
       <c r="J36" s="1">
         <v>0</v>
       </c>
-      <c r="K36" s="7">
+      <c r="K36" s="6">
         <v>15.036</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S36" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="T36" s="1" t="s">
+      <c r="M36" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="U36" s="2" t="s">
+      <c r="N36" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:21">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -3228,23 +3108,20 @@
       <c r="J37" s="1">
         <v>0</v>
       </c>
-      <c r="K37" s="7">
+      <c r="K37" s="6">
         <v>15.036</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S37" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="T37" s="1" t="s">
+      <c r="M37" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="U37" s="2" t="s">
+      <c r="N37" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:21">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -3275,23 +3152,20 @@
       <c r="J38" s="1">
         <v>1</v>
       </c>
-      <c r="K38" s="7">
+      <c r="K38" s="6">
         <v>58.44</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S38" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="T38" s="1" t="s">
+      <c r="M38" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="U38" s="2" t="s">
+      <c r="N38" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:21">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -3313,32 +3187,29 @@
       <c r="G39" s="1">
         <v>0</v>
       </c>
-      <c r="H39" s="6">
-        <v>0</v>
-      </c>
-      <c r="I39" s="6">
-        <v>0</v>
-      </c>
-      <c r="J39" s="6">
-        <v>0</v>
-      </c>
-      <c r="K39" s="7">
+      <c r="H39" s="5">
+        <v>0</v>
+      </c>
+      <c r="I39" s="5">
+        <v>0</v>
+      </c>
+      <c r="J39" s="5">
+        <v>0</v>
+      </c>
+      <c r="K39" s="6">
         <v>148.19499999999999</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S39" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="T39" s="1" t="s">
+      <c r="M39" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="U39" s="2" t="s">
+      <c r="N39" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:21">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -3369,23 +3240,20 @@
       <c r="J40" s="1">
         <v>0</v>
       </c>
-      <c r="K40" s="7">
+      <c r="K40" s="6">
         <v>59.116</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S40" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="T40" s="1" t="s">
+      <c r="M40" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="U40" s="2" t="s">
+      <c r="N40" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:21">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -3416,23 +3284,20 @@
       <c r="J41" s="1">
         <v>0</v>
       </c>
-      <c r="K41" s="7">
+      <c r="K41" s="6">
         <v>60.116</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S41" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="T41" s="1" t="s">
+      <c r="M41" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="U41" s="2" t="s">
+      <c r="N41" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:21">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -3463,23 +3328,20 @@
       <c r="J42" s="1">
         <v>0</v>
       </c>
-      <c r="K42" s="7">
+      <c r="K42" s="6">
         <v>391.69400000000002</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S42" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="T42" s="1" t="s">
+      <c r="M42" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="U42" s="2" t="s">
+      <c r="N42" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:21">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -3510,23 +3372,20 @@
       <c r="J43" s="1">
         <v>0</v>
       </c>
-      <c r="K43" s="7">
+      <c r="K43" s="6">
         <v>143.40799999999999</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S43" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="T43" s="1" t="s">
+      <c r="M43" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="U43" s="2" t="s">
+      <c r="N43" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:21">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -3557,23 +3416,20 @@
       <c r="J44" s="1">
         <v>0</v>
       </c>
-      <c r="K44" s="7">
+      <c r="K44" s="6">
         <v>143.40799999999999</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S44" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="T44" s="1" t="s">
+      <c r="M44" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="U44" s="2" t="s">
+      <c r="N44" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:21">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -3604,23 +3460,20 @@
       <c r="J45" s="1">
         <v>0</v>
       </c>
-      <c r="K45" s="7">
+      <c r="K45" s="6">
         <v>180.15600000000001</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S45" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="T45" s="1" t="s">
+      <c r="M45" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="U45" s="2" t="s">
+      <c r="N45" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:21">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -3651,23 +3504,20 @@
       <c r="J46" s="1">
         <v>0</v>
       </c>
-      <c r="K46" s="7">
+      <c r="K46" s="6">
         <v>89.093999999999994</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S46" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="T46" s="1" t="s">
+      <c r="M46" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="U46" s="2" t="s">
+      <c r="N46" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:21">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3698,23 +3548,20 @@
       <c r="J47" s="1">
         <v>0</v>
       </c>
-      <c r="K47" s="7">
+      <c r="K47" s="6">
         <v>174.20400000000001</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S47" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="T47" s="1" t="s">
+      <c r="M47" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="U47" s="2" t="s">
+      <c r="N47" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:21">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -3745,23 +3592,20 @@
       <c r="J48" s="1">
         <v>0</v>
       </c>
-      <c r="K48" s="7">
+      <c r="K48" s="6">
         <v>132.119</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S48" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="T48" s="1" t="s">
+      <c r="M48" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="U48" s="2" t="s">
+      <c r="N48" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:21">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3792,23 +3636,20 @@
       <c r="J49" s="1">
         <v>0</v>
       </c>
-      <c r="K49" s="7">
+      <c r="K49" s="6">
         <v>133.10300000000001</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S49" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="T49" s="1" t="s">
+      <c r="M49" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="U49" s="2" t="s">
+      <c r="N49" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:21">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3839,23 +3680,20 @@
       <c r="J50" s="1">
         <v>0</v>
       </c>
-      <c r="K50" s="7">
+      <c r="K50" s="6">
         <v>121.154</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S50" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="T50" s="1" t="s">
+      <c r="M50" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="U50" s="2" t="s">
+      <c r="N50" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:21">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3886,23 +3724,20 @@
       <c r="J51" s="1">
         <v>0</v>
       </c>
-      <c r="K51" s="7">
+      <c r="K51" s="6">
         <v>147.13</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S51" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="T51" s="1" t="s">
+      <c r="M51" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="U51" s="2" t="s">
+      <c r="N51" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:21">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3933,23 +3768,20 @@
       <c r="J52" s="1">
         <v>0</v>
       </c>
-      <c r="K52" s="7">
+      <c r="K52" s="6">
         <v>146.14599999999999</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S52" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="T52" s="1" t="s">
+      <c r="M52" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="U52" s="2" t="s">
+      <c r="N52" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:21">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3980,23 +3812,20 @@
       <c r="J53" s="1">
         <v>0</v>
       </c>
-      <c r="K53" s="7">
+      <c r="K53" s="6">
         <v>75.066999999999993</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S53" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="T53" s="1" t="s">
+      <c r="M53" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="U53" s="2" t="s">
+      <c r="N53" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:21">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -4027,23 +3856,20 @@
       <c r="J54" s="1">
         <v>0</v>
       </c>
-      <c r="K54" s="7">
+      <c r="K54" s="6">
         <v>155.15700000000001</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S54" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="T54" s="1" t="s">
+      <c r="M54" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="U54" s="2" t="s">
+      <c r="N54" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:21">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -4074,23 +3900,20 @@
       <c r="J55" s="1">
         <v>0</v>
       </c>
-      <c r="K55" s="7">
+      <c r="K55" s="6">
         <v>46.069000000000003</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S55" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="T55" s="1" t="s">
+      <c r="M55" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="U55" s="2" t="s">
+      <c r="N55" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:21">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -4121,23 +3944,20 @@
       <c r="J56" s="1">
         <v>0</v>
       </c>
-      <c r="K56" s="7">
+      <c r="K56" s="6">
         <v>85.15</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S56" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="T56" s="1" t="s">
+      <c r="M56" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="U56" s="2" t="s">
+      <c r="N56" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:21">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -4168,23 +3988,20 @@
       <c r="J57" s="1">
         <v>0</v>
       </c>
-      <c r="K57" s="7">
+      <c r="K57" s="6">
         <v>310.61</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S57" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="T57" s="1" t="s">
+      <c r="M57" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="U57" s="2" t="s">
+      <c r="N57" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:21">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -4215,23 +4032,20 @@
       <c r="J58" s="1">
         <v>0</v>
       </c>
-      <c r="K58" s="7">
+      <c r="K58" s="6">
         <v>188.69499999999999</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S58" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="T58" s="1" t="s">
+      <c r="M58" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="U58" s="2" t="s">
+      <c r="N58" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:21">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -4262,23 +4076,20 @@
       <c r="J59" s="1">
         <v>0</v>
       </c>
-      <c r="K59" s="7">
+      <c r="K59" s="6">
         <v>154.209</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S59" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="T59" s="1" t="s">
+      <c r="M59" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="U59" s="2" t="s">
+      <c r="N59" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:21">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -4309,23 +4120,20 @@
       <c r="J60" s="1">
         <v>0</v>
       </c>
-      <c r="K60" s="7">
+      <c r="K60" s="6">
         <v>150.64599999999999</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S60" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="T60" s="1" t="s">
+      <c r="M60" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="U60" s="2" t="s">
+      <c r="N60" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:21">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -4356,23 +4164,20 @@
       <c r="J61" s="1">
         <v>0</v>
       </c>
-      <c r="K61" s="7">
+      <c r="K61" s="6">
         <v>170.25200000000001</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S61" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="T61" s="1" t="s">
+      <c r="M61" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="U61" s="2" t="s">
+      <c r="N61" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:21">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -4403,23 +4208,20 @@
       <c r="J62" s="1">
         <v>0</v>
       </c>
-      <c r="K62" s="7">
+      <c r="K62" s="6">
         <v>131.17500000000001</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S62" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="T62" s="1" t="s">
+      <c r="M62" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="U62" s="2" t="s">
+      <c r="N62" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:21">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -4450,35 +4252,1372 @@
       <c r="J63" s="1">
         <v>0</v>
       </c>
-      <c r="K63" s="7">
+      <c r="K63" s="6">
         <v>372.447</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="S63" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="T63" s="1" t="s">
+      <c r="M63" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="U63" s="2" t="s">
+      <c r="N63" s="2" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="K1:L1"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V18" sqref="V18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.83203125" style="34" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="32" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" style="12" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" style="10" customWidth="1"/>
+    <col min="12" max="12" width="6.33203125" style="12" customWidth="1"/>
+    <col min="13" max="13" width="6.33203125" style="10" customWidth="1"/>
+    <col min="14" max="14" width="6.33203125" style="12" customWidth="1"/>
+    <col min="15" max="15" width="6.33203125" style="10" customWidth="1"/>
+    <col min="16" max="16" width="6.33203125" style="12" customWidth="1"/>
+    <col min="17" max="17" width="6.33203125" style="10" customWidth="1"/>
+    <col min="18" max="18" width="6.33203125" style="12" customWidth="1"/>
+    <col min="19" max="19" width="6.33203125" style="29" customWidth="1"/>
+    <col min="20" max="21" width="6.33203125" style="10" customWidth="1"/>
+    <col min="22" max="22" width="52.6640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="10.83203125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="22"/>
+      <c r="F1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="U1" s="16"/>
+      <c r="V1" s="18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="33"/>
+      <c r="B2" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="T2" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="U2" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="V2" s="19"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" s="34">
+        <v>1</v>
+      </c>
+      <c r="D3" s="24">
+        <v>72.150999999999996</v>
+      </c>
+      <c r="E3" s="21">
+        <v>72.148300000000006</v>
+      </c>
+      <c r="F3" s="11">
+        <v>2.19</v>
+      </c>
+      <c r="G3" s="10">
+        <v>0.54765242179106199</v>
+      </c>
+      <c r="H3" s="11">
+        <v>6.42</v>
+      </c>
+      <c r="I3" s="9">
+        <v>6.4166666666666599</v>
+      </c>
+      <c r="J3" s="11">
+        <v>35</v>
+      </c>
+      <c r="K3" s="9">
+        <v>35</v>
+      </c>
+      <c r="L3" s="12">
+        <v>6</v>
+      </c>
+      <c r="N3" s="12">
+        <v>2.41</v>
+      </c>
+      <c r="O3" s="10">
+        <v>2.41421356237309</v>
+      </c>
+      <c r="P3" s="12">
+        <v>20</v>
+      </c>
+      <c r="R3" s="11">
+        <v>20</v>
+      </c>
+      <c r="S3" s="28">
+        <v>20</v>
+      </c>
+      <c r="T3" s="9">
+        <v>2</v>
+      </c>
+      <c r="U3" s="9"/>
+      <c r="V3" s="27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" s="34">
+        <v>2</v>
+      </c>
+      <c r="D4" s="24">
+        <v>72.150999999999996</v>
+      </c>
+      <c r="F4" s="11">
+        <v>2.54</v>
+      </c>
+      <c r="G4" s="10">
+        <v>0.59664809680219799</v>
+      </c>
+      <c r="H4" s="11">
+        <v>6.67</v>
+      </c>
+      <c r="I4" s="9">
+        <v>6.6666666666666599</v>
+      </c>
+      <c r="J4" s="11">
+        <v>28</v>
+      </c>
+      <c r="K4" s="9">
+        <v>28</v>
+      </c>
+      <c r="L4" s="12">
+        <v>8</v>
+      </c>
+      <c r="N4" s="12">
+        <v>2.27</v>
+      </c>
+      <c r="O4" s="10">
+        <v>2.2700556100296598</v>
+      </c>
+      <c r="P4" s="12">
+        <v>18</v>
+      </c>
+      <c r="R4" s="11">
+        <v>18</v>
+      </c>
+      <c r="S4" s="28">
+        <v>18</v>
+      </c>
+      <c r="T4" s="9">
+        <v>2</v>
+      </c>
+      <c r="U4" s="9"/>
+      <c r="V4" s="27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" s="34">
+        <v>3</v>
+      </c>
+      <c r="D5" s="24">
+        <v>72.150999999999996</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="9">
+        <v>7</v>
+      </c>
+      <c r="J5" s="11"/>
+      <c r="K5" s="9">
+        <v>22</v>
+      </c>
+      <c r="R5" s="11"/>
+      <c r="S5" s="28">
+        <v>16</v>
+      </c>
+      <c r="T5" s="9"/>
+      <c r="U5" s="9"/>
+      <c r="V5" s="27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" s="34">
+        <v>4</v>
+      </c>
+      <c r="D6" s="24">
+        <v>56.107999999999997</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="9">
+        <v>4.33</v>
+      </c>
+      <c r="J6" s="11"/>
+      <c r="K6" s="9">
+        <v>15</v>
+      </c>
+      <c r="R6" s="11"/>
+      <c r="S6" s="28">
+        <v>10</v>
+      </c>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" s="34">
+        <v>5</v>
+      </c>
+      <c r="D7" s="24">
+        <v>56.107999999999997</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="9">
+        <v>4.33</v>
+      </c>
+      <c r="J7" s="11"/>
+      <c r="K7" s="9">
+        <v>15</v>
+      </c>
+      <c r="R7" s="11"/>
+      <c r="S7" s="28">
+        <v>10</v>
+      </c>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" s="34">
+        <v>6</v>
+      </c>
+      <c r="D8" s="24">
+        <v>56.107999999999997</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8" s="9">
+        <v>4.33</v>
+      </c>
+      <c r="J8" s="11"/>
+      <c r="K8" s="9">
+        <v>15</v>
+      </c>
+      <c r="R8" s="11"/>
+      <c r="S8" s="28">
+        <v>10</v>
+      </c>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" s="34">
+        <v>7</v>
+      </c>
+      <c r="D9" s="24">
+        <v>56.107999999999997</v>
+      </c>
+      <c r="H9" s="11"/>
+      <c r="I9" s="9">
+        <v>4.33</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="9">
+        <v>15</v>
+      </c>
+      <c r="R9" s="11"/>
+      <c r="S9" s="28">
+        <v>10</v>
+      </c>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" s="34">
+        <v>8</v>
+      </c>
+      <c r="D10" s="24">
+        <v>54.091999999999999</v>
+      </c>
+      <c r="H10" s="11"/>
+      <c r="I10" s="9">
+        <v>4.33</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="9">
+        <v>15</v>
+      </c>
+      <c r="R10" s="11"/>
+      <c r="S10" s="28">
+        <v>10</v>
+      </c>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" s="34">
+        <v>9</v>
+      </c>
+      <c r="D11" s="24">
+        <v>54.091999999999999</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="9">
+        <v>4.33</v>
+      </c>
+      <c r="J11" s="11"/>
+      <c r="K11" s="9">
+        <v>15</v>
+      </c>
+      <c r="R11" s="11"/>
+      <c r="S11" s="28">
+        <v>10</v>
+      </c>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12" s="34">
+        <v>10</v>
+      </c>
+      <c r="D12" s="24">
+        <v>54.091999999999999</v>
+      </c>
+      <c r="H12" s="11"/>
+      <c r="I12" s="9">
+        <v>4.33</v>
+      </c>
+      <c r="J12" s="11"/>
+      <c r="K12" s="9">
+        <v>15</v>
+      </c>
+      <c r="R12" s="11"/>
+      <c r="S12" s="28">
+        <v>10</v>
+      </c>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" s="34">
+        <v>11</v>
+      </c>
+      <c r="D13" s="24">
+        <v>54.091999999999999</v>
+      </c>
+      <c r="H13" s="11"/>
+      <c r="I13" s="9">
+        <v>4.33</v>
+      </c>
+      <c r="J13" s="11"/>
+      <c r="K13" s="9">
+        <v>15</v>
+      </c>
+      <c r="R13" s="11"/>
+      <c r="S13" s="28">
+        <v>10</v>
+      </c>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14" s="34">
+        <v>12</v>
+      </c>
+      <c r="D14" s="24">
+        <v>74.123000000000005</v>
+      </c>
+      <c r="H14" s="11"/>
+      <c r="I14" s="9">
+        <v>6.42</v>
+      </c>
+      <c r="J14" s="11"/>
+      <c r="K14" s="9">
+        <v>35</v>
+      </c>
+      <c r="R14" s="11"/>
+      <c r="S14" s="28">
+        <v>20</v>
+      </c>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" s="34">
+        <v>13</v>
+      </c>
+      <c r="D15" s="24">
+        <v>74.123000000000005</v>
+      </c>
+      <c r="H15" s="11"/>
+      <c r="I15" s="9">
+        <v>6.67</v>
+      </c>
+      <c r="J15" s="11"/>
+      <c r="K15" s="9">
+        <v>28</v>
+      </c>
+      <c r="R15" s="11"/>
+      <c r="S15" s="28">
+        <v>18</v>
+      </c>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16" s="34">
+        <v>14</v>
+      </c>
+      <c r="D16" s="24">
+        <v>74.123000000000005</v>
+      </c>
+      <c r="H16" s="11"/>
+      <c r="I16" s="9">
+        <v>7</v>
+      </c>
+      <c r="J16" s="11"/>
+      <c r="K16" s="9">
+        <v>22</v>
+      </c>
+      <c r="R16" s="11"/>
+      <c r="S16" s="28">
+        <v>16</v>
+      </c>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A17" s="34">
+        <v>15</v>
+      </c>
+      <c r="D17" s="24">
+        <v>72.106999999999999</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" s="9">
+        <v>6.42</v>
+      </c>
+      <c r="J17" s="11"/>
+      <c r="K17" s="9">
+        <v>35</v>
+      </c>
+      <c r="R17" s="11"/>
+      <c r="S17" s="28">
+        <v>20</v>
+      </c>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A18" s="34">
+        <v>16</v>
+      </c>
+      <c r="D18" s="24">
+        <v>72.106999999999999</v>
+      </c>
+      <c r="V18" s="27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A19" s="34">
+        <v>17</v>
+      </c>
+      <c r="D19" s="24">
+        <v>88.105999999999995</v>
+      </c>
+      <c r="V19" s="27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A20" s="34">
+        <v>18</v>
+      </c>
+      <c r="D20" s="24">
+        <v>88.105999999999995</v>
+      </c>
+      <c r="V20" s="27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A21" s="34">
+        <v>19</v>
+      </c>
+      <c r="D21" s="24">
+        <v>87.122</v>
+      </c>
+      <c r="V21" s="27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A22" s="34">
+        <v>20</v>
+      </c>
+      <c r="D22" s="24">
+        <v>104.105</v>
+      </c>
+      <c r="V22" s="27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A23" s="34">
+        <v>21</v>
+      </c>
+      <c r="D23" s="24">
+        <v>106.54900000000001</v>
+      </c>
+      <c r="V23" s="27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A24" s="34">
+        <v>22</v>
+      </c>
+      <c r="D24" s="24">
+        <v>116.116</v>
+      </c>
+      <c r="V24" s="27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A25" s="34">
+        <v>23</v>
+      </c>
+      <c r="D25" s="24">
+        <v>84.162000000000006</v>
+      </c>
+      <c r="V25" s="27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A26" s="34">
+        <v>24</v>
+      </c>
+      <c r="D26" s="24">
+        <v>166.30799999999999</v>
+      </c>
+      <c r="V26" s="27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A27" s="34">
+        <v>25</v>
+      </c>
+      <c r="D27" s="24">
+        <v>152.28100000000001</v>
+      </c>
+      <c r="V27" s="27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A28" s="34">
+        <v>26</v>
+      </c>
+      <c r="D28" s="24">
+        <v>80.13</v>
+      </c>
+      <c r="V28" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A29" s="34">
+        <v>27</v>
+      </c>
+      <c r="D29" s="24">
+        <v>104.152</v>
+      </c>
+      <c r="V29" s="27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A30" s="34">
+        <v>28</v>
+      </c>
+      <c r="D30" s="24">
+        <v>78.114000000000004</v>
+      </c>
+      <c r="V30" s="27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A31" s="34">
+        <v>29</v>
+      </c>
+      <c r="D31" s="24">
+        <v>108.14</v>
+      </c>
+      <c r="V31" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A32" s="34">
+        <v>30</v>
+      </c>
+      <c r="D32" s="24">
+        <v>154.21199999999999</v>
+      </c>
+      <c r="V32" s="27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A33" s="34">
+        <v>31</v>
+      </c>
+      <c r="D33" s="24">
+        <v>178.22300000000001</v>
+      </c>
+      <c r="V33" s="27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A34" s="34">
+        <v>32</v>
+      </c>
+      <c r="D34" s="24">
+        <v>67.090999999999994</v>
+      </c>
+      <c r="V34" s="27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A35" s="34">
+        <v>33</v>
+      </c>
+      <c r="D35" s="24">
+        <v>68.075000000000003</v>
+      </c>
+      <c r="V35" s="27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A36" s="34">
+        <v>34</v>
+      </c>
+      <c r="D36" s="24">
+        <v>84.135999999999996</v>
+      </c>
+      <c r="V36" s="27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A37" s="34">
+        <v>35</v>
+      </c>
+      <c r="D37" s="24">
+        <v>15.036</v>
+      </c>
+      <c r="V37" s="27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A38" s="34">
+        <v>36</v>
+      </c>
+      <c r="D38" s="24">
+        <v>15.036</v>
+      </c>
+      <c r="V38" s="27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A39" s="34">
+        <v>37</v>
+      </c>
+      <c r="D39" s="24">
+        <v>58.44</v>
+      </c>
+      <c r="V39" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A40" s="34">
+        <v>38</v>
+      </c>
+      <c r="D40" s="24">
+        <v>148.19499999999999</v>
+      </c>
+      <c r="V40" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A41" s="34">
+        <v>39</v>
+      </c>
+      <c r="D41" s="24">
+        <v>59.116</v>
+      </c>
+      <c r="V41" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A42" s="34">
+        <v>40</v>
+      </c>
+      <c r="D42" s="24">
+        <v>60.116</v>
+      </c>
+      <c r="V42" s="27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A43" s="34">
+        <v>41</v>
+      </c>
+      <c r="D43" s="24">
+        <v>391.69400000000002</v>
+      </c>
+      <c r="V43" s="27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A44" s="34">
+        <v>42</v>
+      </c>
+      <c r="D44" s="24">
+        <v>143.40799999999999</v>
+      </c>
+      <c r="V44" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A45" s="34">
+        <v>43</v>
+      </c>
+      <c r="D45" s="24">
+        <v>143.40799999999999</v>
+      </c>
+      <c r="V45" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A46" s="34">
+        <v>44</v>
+      </c>
+      <c r="D46" s="24">
+        <v>180.15600000000001</v>
+      </c>
+      <c r="V46" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A47" s="34">
+        <v>45</v>
+      </c>
+      <c r="D47" s="24">
+        <v>89.093999999999994</v>
+      </c>
+      <c r="V47" s="27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A48" s="34">
+        <v>46</v>
+      </c>
+      <c r="D48" s="24">
+        <v>174.20400000000001</v>
+      </c>
+      <c r="V48" s="27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A49" s="34">
+        <v>47</v>
+      </c>
+      <c r="D49" s="24">
+        <v>132.119</v>
+      </c>
+      <c r="V49" s="27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A50" s="34">
+        <v>48</v>
+      </c>
+      <c r="D50" s="24">
+        <v>133.10300000000001</v>
+      </c>
+      <c r="V50" s="27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A51" s="34">
+        <v>49</v>
+      </c>
+      <c r="D51" s="24">
+        <v>121.154</v>
+      </c>
+      <c r="V51" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A52" s="34">
+        <v>50</v>
+      </c>
+      <c r="D52" s="24">
+        <v>147.13</v>
+      </c>
+      <c r="V52" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A53" s="34">
+        <v>51</v>
+      </c>
+      <c r="D53" s="24">
+        <v>146.14599999999999</v>
+      </c>
+      <c r="V53" s="27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A54" s="34">
+        <v>52</v>
+      </c>
+      <c r="D54" s="24">
+        <v>75.066999999999993</v>
+      </c>
+      <c r="V54" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A55" s="34">
+        <v>53</v>
+      </c>
+      <c r="D55" s="24">
+        <v>155.15700000000001</v>
+      </c>
+      <c r="V55" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A56" s="34">
+        <v>54</v>
+      </c>
+      <c r="D56" s="24">
+        <v>46.069000000000003</v>
+      </c>
+      <c r="V56" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A57" s="34">
+        <v>55</v>
+      </c>
+      <c r="D57" s="24">
+        <v>85.15</v>
+      </c>
+      <c r="V57" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A58" s="34">
+        <v>56</v>
+      </c>
+      <c r="D58" s="24">
+        <v>310.61</v>
+      </c>
+      <c r="V58" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A59" s="34">
+        <v>57</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D59" s="24">
+        <v>188.69499999999999</v>
+      </c>
+      <c r="E59" s="21">
+        <v>188.69069999999999</v>
+      </c>
+      <c r="F59" s="11">
+        <v>3.85</v>
+      </c>
+      <c r="G59" s="10">
+        <v>0.32905000000000001</v>
+      </c>
+      <c r="H59" s="12">
+        <v>28.42</v>
+      </c>
+      <c r="I59" s="10">
+        <v>28.416599999999999</v>
+      </c>
+      <c r="J59" s="12">
+        <v>523</v>
+      </c>
+      <c r="K59" s="10">
+        <v>523</v>
+      </c>
+      <c r="L59" s="12">
+        <v>28</v>
+      </c>
+      <c r="N59" s="12">
+        <v>5.49</v>
+      </c>
+      <c r="O59" s="10">
+        <v>5.4852689999999997</v>
+      </c>
+      <c r="P59" s="12">
+        <v>211</v>
+      </c>
+      <c r="R59" s="12">
+        <v>211</v>
+      </c>
+      <c r="S59" s="29">
+        <v>211</v>
+      </c>
+      <c r="T59" s="10">
+        <v>14</v>
+      </c>
+      <c r="V59" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A60" s="34">
+        <v>58</v>
+      </c>
+      <c r="B60" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D60" s="24">
+        <v>154.209</v>
+      </c>
+      <c r="E60" s="21">
+        <v>154.20570000000001</v>
+      </c>
+      <c r="F60" s="11">
+        <v>1.99</v>
+      </c>
+      <c r="G60" s="10">
+        <v>0.402918</v>
+      </c>
+      <c r="H60" s="12">
+        <v>27.85</v>
+      </c>
+      <c r="I60" s="10">
+        <v>27.85</v>
+      </c>
+      <c r="J60" s="12">
+        <v>285</v>
+      </c>
+      <c r="K60" s="10">
+        <v>285</v>
+      </c>
+      <c r="L60" s="12">
+        <v>32</v>
+      </c>
+      <c r="N60" s="12">
+        <v>5.38</v>
+      </c>
+      <c r="O60" s="10">
+        <v>5.3769999999999998</v>
+      </c>
+      <c r="P60" s="12">
+        <v>300</v>
+      </c>
+      <c r="R60" s="12">
+        <v>140</v>
+      </c>
+      <c r="S60" s="29">
+        <v>140</v>
+      </c>
+      <c r="T60" s="10">
+        <v>15</v>
+      </c>
+      <c r="V60" s="27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A61" s="34">
+        <v>59</v>
+      </c>
+      <c r="B61" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D61" s="24">
+        <v>150.64599999999999</v>
+      </c>
+      <c r="E61" s="21">
+        <v>150.64279999999999</v>
+      </c>
+      <c r="F61" s="11">
+        <v>3.15</v>
+      </c>
+      <c r="G61" s="10">
+        <v>0.37592088566814003</v>
+      </c>
+      <c r="H61" s="12">
+        <v>17.52</v>
+      </c>
+      <c r="I61" s="10">
+        <v>17.516666666666602</v>
+      </c>
+      <c r="J61" s="12">
+        <v>234</v>
+      </c>
+      <c r="K61" s="10">
+        <v>234</v>
+      </c>
+      <c r="L61" s="12">
+        <v>18</v>
+      </c>
+      <c r="N61" s="12">
+        <v>4.16</v>
+      </c>
+      <c r="O61" s="10">
+        <v>4.1639024601470096</v>
+      </c>
+      <c r="P61" s="12">
+        <v>102</v>
+      </c>
+      <c r="R61" s="12">
+        <v>102</v>
+      </c>
+      <c r="S61" s="29">
+        <v>102</v>
+      </c>
+      <c r="T61" s="10">
+        <v>7</v>
+      </c>
+      <c r="V61" s="27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A62" s="34">
+        <v>60</v>
+      </c>
+      <c r="B62" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="C62" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="D62" s="21">
+        <v>170.25200000000001</v>
+      </c>
+      <c r="E62" s="21">
+        <v>170.24799999999999</v>
+      </c>
+      <c r="F62" s="11">
+        <v>2.42</v>
+      </c>
+      <c r="G62" s="10">
+        <v>0.35281000000000001</v>
+      </c>
+      <c r="H62" s="12">
+        <v>30.09</v>
+      </c>
+      <c r="I62" s="10">
+        <v>30.092849999999999</v>
+      </c>
+      <c r="J62" s="12">
+        <v>468</v>
+      </c>
+      <c r="K62" s="10">
+        <v>468</v>
+      </c>
+      <c r="L62" s="12">
+        <v>32</v>
+      </c>
+      <c r="N62" s="12">
+        <v>5.65</v>
+      </c>
+      <c r="O62" s="10">
+        <v>5.6470657077414002</v>
+      </c>
+      <c r="P62" s="12">
+        <v>303</v>
+      </c>
+      <c r="R62" s="12">
+        <v>197</v>
+      </c>
+      <c r="S62" s="29">
+        <v>197</v>
+      </c>
+      <c r="T62" s="10">
+        <v>16</v>
+      </c>
+      <c r="V62" s="27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A63" s="34">
+        <v>61</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D63" s="24">
+        <v>131.18</v>
+      </c>
+      <c r="E63" s="21">
+        <v>131.17240000000001</v>
+      </c>
+      <c r="F63" s="11">
+        <v>3.58</v>
+      </c>
+      <c r="G63" s="10">
+        <v>0.41200922530448503</v>
+      </c>
+      <c r="H63" s="12">
+        <v>18.23</v>
+      </c>
+      <c r="I63" s="10">
+        <v>18.233333333333299</v>
+      </c>
+      <c r="J63" s="12">
+        <v>188</v>
+      </c>
+      <c r="K63" s="10">
+        <v>188</v>
+      </c>
+      <c r="L63" s="12">
+        <v>20</v>
+      </c>
+      <c r="N63" s="12">
+        <v>4.09</v>
+      </c>
+      <c r="O63" s="10">
+        <v>4.09142281507558</v>
+      </c>
+      <c r="P63" s="12">
+        <v>92</v>
+      </c>
+      <c r="R63" s="12">
+        <v>92</v>
+      </c>
+      <c r="S63" s="29">
+        <v>92</v>
+      </c>
+      <c r="T63" s="10">
+        <v>10</v>
+      </c>
+      <c r="V63" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A64" s="34">
+        <v>62</v>
+      </c>
+      <c r="D64" s="24">
+        <v>372.447</v>
+      </c>
+      <c r="V64" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>